<commit_message>
update social feeds/jobs/training page
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tj_hou/Documents/ESG_Project/ESG_website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7167B2DC-CA9D-2D44-8E8D-03C37496442A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6393108F-900C-7241-8CC9-6A08B25DFE48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="20720" windowHeight="13280" tabRatio="767" firstSheet="8" activeTab="18" xr2:uid="{21188EBB-03F7-4643-B426-6DBAB4FD05DB}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="20720" windowHeight="13280" tabRatio="767" firstSheet="8" activeTab="13" xr2:uid="{21188EBB-03F7-4643-B426-6DBAB4FD05DB}"/>
   </bookViews>
   <sheets>
     <sheet name="arxiv" sheetId="1" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="243">
   <si>
     <t>Title</t>
   </si>
@@ -835,6 +835,42 @@
   </si>
   <si>
     <t>Training</t>
+  </si>
+  <si>
+    <t>https://www.icgn.org/education</t>
+  </si>
+  <si>
+    <t>courses, in-house training, academic days and publications</t>
+  </si>
+  <si>
+    <t>ICGN</t>
+  </si>
+  <si>
+    <t>encouraging best practice and informing members about key developments in corporate governance and investor stewardship</t>
+  </si>
+  <si>
+    <t>https://sustainability-academy.org/</t>
+  </si>
+  <si>
+    <t>certified online courses</t>
+  </si>
+  <si>
+    <t>Sustainability Academy</t>
+  </si>
+  <si>
+    <t>keep up to date with current legislation, global trends and best cases of Sustainability and Corporate Responsibility</t>
+  </si>
+  <si>
+    <t>https://www.ussif.org/courses</t>
+  </si>
+  <si>
+    <t>USSIF</t>
+  </si>
+  <si>
+    <t>courses</t>
+  </si>
+  <si>
+    <t>Sustainable Investment, Fundamentals of Sustainable and Impact Investment,Chartered SRI CounselorSM (CSRIC®)</t>
   </si>
 </sst>
 </file>
@@ -1533,12 +1569,12 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.6640625" customWidth="1"/>
+    <col min="1" max="1" width="97.6640625" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.1640625" customWidth="1"/>
   </cols>
@@ -1639,13 +1675,17 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E50B0918-D333-4FAA-A239-B24EBC51EF6F}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="29" customWidth="1"/>
+    <col min="2" max="2" width="56" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -1689,8 +1729,55 @@
         <v>99</v>
       </c>
     </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>232</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>231</v>
+      </c>
+      <c r="C4" t="s">
+        <v>233</v>
+      </c>
+      <c r="D4" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>236</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>235</v>
+      </c>
+      <c r="C5" t="s">
+        <v>237</v>
+      </c>
+      <c r="D5" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>241</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>239</v>
+      </c>
+      <c r="C6" t="s">
+        <v>240</v>
+      </c>
+      <c r="D6" t="s">
+        <v>242</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="B4" r:id="rId1" xr:uid="{F1A5D0A2-673E-304F-A897-067FEE624982}"/>
+    <hyperlink ref="B5" r:id="rId2" xr:uid="{1CBAF31D-F364-6243-94A5-212EBD76A6D1}"/>
+    <hyperlink ref="B6" r:id="rId3" xr:uid="{BEC593FE-19A8-534E-A3D2-6264F07CC3B6}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2055,8 +2142,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{708919BB-1ECF-C149-90E6-4514E4E287A9}">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>